<commit_message>
Añadidos diagramas de cajas y bigotes
</commit_message>
<xml_diff>
--- a/informe/Mutación.xlsx
+++ b/informe/Mutación.xlsx
@@ -9,6 +9,32 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Hoja1!$R$6</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Hoja1!$R$7:$R$11</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Hoja1!$T$20</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Hoja1!$T$21:$T$25</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Hoja1!$R$20</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Hoja1!$R$21:$R$25</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Hoja1!$S$20</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Hoja1!$S$21:$S$25</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Hoja1!$T$20</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Hoja1!$T$21:$T$25</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Hoja1!$R$13</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Hoja1!$R$14:$R$18</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Hoja1!$S$6</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Hoja1!$S$13</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Hoja1!$S$14:$S$18</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Hoja1!$T$13</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Hoja1!$T$14:$T$18</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Hoja1!$S$7:$S$11</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Hoja1!$T$6</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Hoja1!$T$7:$T$11</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Hoja1!$R$20</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Hoja1!$R$21:$R$25</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Hoja1!$S$20</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Hoja1!$S$21:$S$25</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>SOM-1</t>
   </si>
@@ -226,7 +252,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.11938888888888889"/>
-          <c:y val="3.7037037037037035E-2"/>
+          <c:y val="4.1666666666666664E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -658,7 +684,412 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.1</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.3</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.5</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>SOM-b_11</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{DD27AE94-DE5A-4F70-8CAB-B0CFF5DFB73E}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:v>Mutación 0,01</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{11760D70-32F1-465B-81CC-152EDEC3FD1E}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:v>Mutación 0,05</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{43BA550C-4331-46B3-9098-FA786D531C6D}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:v>Mutación 0,09</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="b" align="ctr" overlay="0"/>
+  </cx:chart>
+  <cx:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.19</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.21</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.23</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>SOM-b_12</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{6944AAF2-00B5-4796-B539-E22CDD972BE9}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.18</cx:f>
+              <cx:v>Mutación 0,01</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{29CBF583-4F27-471A-8FD7-2413BA363404}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:v>Mutación 0,05</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{2ED0BBEE-508C-4D99-988B-81BB7E81C461}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:v>Mutación 0,09</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="b" align="ctr" overlay="0"/>
+  </cx:chart>
+  <cx:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.13</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.15</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.17</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-ES"/>
+              <a:t>SOM-b_13</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{69F4648F-678B-4CF2-815B-C3238B3764B1}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:v>Mutación 0,01</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{4539CDDE-8C98-485C-8D36-E537F966E6E9}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:v>Mutación 0,05</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{0499799E-DBD7-4A65-9E46-839655785097}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.16</cx:f>
+              <cx:v>Mutación 0,09</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+    <cx:legend pos="b" align="ctr" overlay="0"/>
+  </cx:chart>
+  <cx:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+</cx:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1201,20 +1632,1463 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="373">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9575" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="sq" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9575" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" i="0" kern="1200" spc="20" baseline="0"/>
+    <cs:bodyPr rot="0" vert="horz"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="373">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9575" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="sq" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9575" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" i="0" kern="1200" spc="20" baseline="0"/>
+    <cs:bodyPr rot="0" vert="horz"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="373">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9575" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+            <a:lumOff val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="sq" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9575" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" i="0" kern="1200" spc="20" baseline="0"/>
+    <cs:bodyPr rot="0" vert="horz"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" spc="20" baseline="0"/>
+    <cs:bodyPr rot="-60000000" vert="horz"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1231,6 +3105,210 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Gráfico 1"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="4" name="Gráfico 3"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>385762</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>61911</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="5" name="Gráfico 4"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1100"/>
+                <a:t>Este gráfico no está disponible en su versión de Excel.
+Si edita esta forma o guarda el libro en un formato de archivo diferente, el gráfico no se podrá utilizar.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1536,10 +3614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D7:O21"/>
+  <dimension ref="D6:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="G24" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,7 +3629,18 @@
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>6</v>
+      </c>
+      <c r="S6" t="s">
+        <v>7</v>
+      </c>
+      <c r="T6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E7" s="1">
         <v>20653</v>
       </c>
@@ -1579,8 +3668,17 @@
       <c r="O7">
         <v>4488</v>
       </c>
+      <c r="R7" s="1">
+        <v>20653</v>
+      </c>
+      <c r="S7">
+        <v>20407</v>
+      </c>
+      <c r="T7">
+        <v>19944</v>
+      </c>
     </row>
-    <row r="8" spans="4:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="1">
         <v>20632</v>
       </c>
@@ -1608,8 +3706,17 @@
       <c r="O8">
         <v>4428</v>
       </c>
+      <c r="R8" s="1">
+        <v>20632</v>
+      </c>
+      <c r="S8">
+        <v>20137</v>
+      </c>
+      <c r="T8">
+        <v>19874</v>
+      </c>
     </row>
-    <row r="9" spans="4:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E9" s="1">
         <v>20538</v>
       </c>
@@ -1637,8 +3744,17 @@
       <c r="O9">
         <v>4466</v>
       </c>
+      <c r="R9" s="1">
+        <v>20538</v>
+      </c>
+      <c r="S9">
+        <v>20345</v>
+      </c>
+      <c r="T9">
+        <v>19907</v>
+      </c>
     </row>
-    <row r="10" spans="4:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="1">
         <v>20574</v>
       </c>
@@ -1666,8 +3782,17 @@
       <c r="O10">
         <v>4447</v>
       </c>
+      <c r="R10" s="1">
+        <v>20574</v>
+      </c>
+      <c r="S10">
+        <v>20234</v>
+      </c>
+      <c r="T10">
+        <v>19785</v>
+      </c>
     </row>
-    <row r="11" spans="4:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E11" s="3">
         <v>20666</v>
       </c>
@@ -1695,8 +3820,17 @@
       <c r="O11">
         <v>4478</v>
       </c>
+      <c r="R11" s="3">
+        <v>20666</v>
+      </c>
+      <c r="S11">
+        <v>20245</v>
+      </c>
+      <c r="T11">
+        <v>19809</v>
+      </c>
     </row>
-    <row r="13" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:20" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>0</v>
       </c>
@@ -1706,8 +3840,17 @@
       <c r="G13" t="s">
         <v>2</v>
       </c>
+      <c r="R13" t="s">
+        <v>6</v>
+      </c>
+      <c r="S13" t="s">
+        <v>7</v>
+      </c>
+      <c r="T13" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="14" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>3</v>
       </c>
@@ -1747,8 +3890,17 @@
         <f>AVERAGE(O7:O11)</f>
         <v>4461.3999999999996</v>
       </c>
+      <c r="R14" s="2">
+        <v>35859</v>
+      </c>
+      <c r="S14">
+        <v>34931</v>
+      </c>
+      <c r="T14">
+        <v>34510</v>
+      </c>
     </row>
-    <row r="15" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>4</v>
       </c>
@@ -1761,8 +3913,17 @@
       <c r="G15">
         <v>4557.3999999999996</v>
       </c>
+      <c r="R15" s="2">
+        <v>35869</v>
+      </c>
+      <c r="S15">
+        <v>35129</v>
+      </c>
+      <c r="T15">
+        <v>34433</v>
+      </c>
     </row>
-    <row r="16" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>5</v>
       </c>
@@ -1775,8 +3936,28 @@
       <c r="G16" s="5">
         <v>4461.3999999999996</v>
       </c>
+      <c r="R16" s="2">
+        <v>35801</v>
+      </c>
+      <c r="S16">
+        <v>35192</v>
+      </c>
+      <c r="T16">
+        <v>34564</v>
+      </c>
     </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R17" s="2">
+        <v>35742</v>
+      </c>
+      <c r="S17">
+        <v>35205</v>
+      </c>
+      <c r="T17">
+        <v>34291</v>
+      </c>
+    </row>
+    <row r="18" spans="4:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>6</v>
       </c>
@@ -1786,8 +3967,17 @@
       <c r="G18" t="s">
         <v>8</v>
       </c>
+      <c r="R18" s="4">
+        <v>35730</v>
+      </c>
+      <c r="S18">
+        <v>34931</v>
+      </c>
+      <c r="T18">
+        <v>34436</v>
+      </c>
     </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>9</v>
       </c>
@@ -1804,7 +3994,7 @@
         <v>2.9970991757181369</v>
       </c>
     </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>10</v>
       </c>
@@ -1829,8 +4019,17 @@
       <c r="N20">
         <v>4658</v>
       </c>
+      <c r="R20" t="s">
+        <v>6</v>
+      </c>
+      <c r="S20" t="s">
+        <v>7</v>
+      </c>
+      <c r="T20" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>11</v>
       </c>
@@ -1845,6 +4044,59 @@
       <c r="G21" s="5">
         <f>(STDEV(G16,N20)/N20)*100</f>
         <v>2.9844824641750858</v>
+      </c>
+      <c r="R21" s="1">
+        <v>4526</v>
+      </c>
+      <c r="S21">
+        <v>4516</v>
+      </c>
+      <c r="T21">
+        <v>4488</v>
+      </c>
+    </row>
+    <row r="22" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R22" s="1">
+        <v>4508</v>
+      </c>
+      <c r="S22">
+        <v>4595</v>
+      </c>
+      <c r="T22">
+        <v>4428</v>
+      </c>
+    </row>
+    <row r="23" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R23" s="1">
+        <v>4578</v>
+      </c>
+      <c r="S23">
+        <v>4581</v>
+      </c>
+      <c r="T23">
+        <v>4466</v>
+      </c>
+    </row>
+    <row r="24" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R24" s="1">
+        <v>4567</v>
+      </c>
+      <c r="S24">
+        <v>4552</v>
+      </c>
+      <c r="T24">
+        <v>4447</v>
+      </c>
+    </row>
+    <row r="25" spans="4:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R25" s="3">
+        <v>4612</v>
+      </c>
+      <c r="S25">
+        <v>4543</v>
+      </c>
+      <c r="T25">
+        <v>4478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Efectos de la probabilidad de cruce
</commit_message>
<xml_diff>
--- a/informe/Mutación.xlsx
+++ b/informe/Mutación.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,28 +12,22 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Hoja1!$R$6</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Hoja1!$R$7:$R$11</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Hoja1!$T$20</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Hoja1!$T$21:$T$25</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Hoja1!$T$13</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Hoja1!$T$14:$T$18</definedName>
     <definedName name="_xlchart.v1.12" hidden="1">Hoja1!$R$20</definedName>
     <definedName name="_xlchart.v1.13" hidden="1">Hoja1!$R$21:$R$25</definedName>
     <definedName name="_xlchart.v1.14" hidden="1">Hoja1!$S$20</definedName>
     <definedName name="_xlchart.v1.15" hidden="1">Hoja1!$S$21:$S$25</definedName>
     <definedName name="_xlchart.v1.16" hidden="1">Hoja1!$T$20</definedName>
     <definedName name="_xlchart.v1.17" hidden="1">Hoja1!$T$21:$T$25</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Hoja1!$R$13</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Hoja1!$R$14:$R$18</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">Hoja1!$S$6</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Hoja1!$S$13</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Hoja1!$S$14:$S$18</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Hoja1!$T$13</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Hoja1!$T$14:$T$18</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">Hoja1!$S$7:$S$11</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">Hoja1!$T$6</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">Hoja1!$T$7:$T$11</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Hoja1!$R$20</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Hoja1!$R$21:$R$25</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Hoja1!$S$20</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Hoja1!$S$21:$S$25</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Hoja1!$R$13</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Hoja1!$R$14:$R$18</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Hoja1!$S$13</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Hoja1!$S$14:$S$18</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -87,7 +81,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +95,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -173,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -188,6 +190,7 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -784,17 +787,17 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.19</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.21</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.23</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -821,7 +824,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{6944AAF2-00B5-4796-B539-E22CDD972BE9}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.18</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>Mutación 0,01</cx:v>
             </cx:txData>
           </cx:tx>
@@ -834,7 +837,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{29CBF583-4F27-471A-8FD7-2413BA363404}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.20</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>Mutación 0,05</cx:v>
             </cx:txData>
           </cx:tx>
@@ -847,7 +850,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{2ED0BBEE-508C-4D99-988B-81BB7E81C461}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>Mutación 0,09</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3616,8 +3619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D6:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G24" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4067,6 +4070,7 @@
       </c>
     </row>
     <row r="23" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H23" s="6"/>
       <c r="R23" s="1">
         <v>4578</v>
       </c>
@@ -4101,6 +4105,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambios en el informe
</commit_message>
<xml_diff>
--- a/informe/Mutación.xlsx
+++ b/informe/Mutación.xlsx
@@ -4,30 +4,44 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Hoja1!$R$6</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Hoja1!$R$7:$R$11</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Hoja1!$T$13</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Hoja1!$T$14:$T$18</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Hoja1!$R$20</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Hoja1!$R$21:$R$25</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Hoja1!$S$20</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Hoja1!$S$21:$S$25</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Hoja1!$T$20</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Hoja1!$T$21:$T$25</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Hoja1!$S$6</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Hoja1!$S$7:$S$11</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Hoja1!$T$6</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Hoja1!$T$7:$T$11</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Hoja1!$R$13</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Hoja1!$R$14:$R$18</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Hoja1!$S$13</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Hoja1!$S$14:$S$18</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Hoja1!$R$20</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Hoja1!$R$21:$R$25</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Hoja1!$S$13</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Hoja1!$S$14:$S$18</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Hoja1!$T$13</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Hoja1!$T$14:$T$18</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Hoja1!$U$13</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Hoja1!$U$14:$U$18</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Hoja1!$R$6</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Hoja1!$R$7:$R$11</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Hoja1!$S$6</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Hoja1!$S$7:$S$11</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Hoja1!$S$20</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Hoja1!$T$6</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Hoja1!$T$7:$T$11</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Hoja1!$U$6</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Hoja1!$U$7:$U$11</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Hoja1!$R$20</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Hoja1!$R$21:$R$25</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Hoja1!$S$20</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Hoja1!$S$21:$S$25</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Hoja1!$T$20</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Hoja1!$T$21:$T$25</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Hoja1!$S$21:$S$25</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Hoja1!$U$20</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Hoja1!$U$21:$U$25</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Hoja1!$T$20</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Hoja1!$T$21:$T$25</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Hoja1!$U$20</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Hoja1!$U$21:$U$25</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Hoja1!$R$13</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Hoja1!$R$14:$R$18</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
   <si>
     <t>SOM-1</t>
   </si>
@@ -76,25 +90,21 @@
   <si>
     <t>SOM-b_13</t>
   </si>
+  <si>
+    <t>Mutación 0,00</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
     </font>
     <font>
       <u/>
@@ -105,68 +115,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -175,22 +135,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -692,17 +640,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.21</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -729,7 +682,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{DD27AE94-DE5A-4F70-8CAB-B0CFF5DFB73E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.16</cx:f>
               <cx:v>Mutación 0,01</cx:v>
             </cx:txData>
           </cx:tx>
@@ -742,7 +695,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{11760D70-32F1-465B-81CC-152EDEC3FD1E}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.18</cx:f>
               <cx:v>Mutación 0,05</cx:v>
             </cx:txData>
           </cx:tx>
@@ -755,13 +708,25 @@
         <cx:series layoutId="boxWhisker" uniqueId="{43BA550C-4331-46B3-9098-FA786D531C6D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.20</cx:f>
               <cx:v>Mutación 0,09</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="2"/>
           <cx:layoutPr>
             <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000000-699B-42D4-A9F9-FADE0702EDC0}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.22</cx:f>
+              <cx:v>Mutación 0,00</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -787,17 +752,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.9</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.11</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -824,7 +794,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{6944AAF2-00B5-4796-B539-E22CDD972BE9}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.6</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>Mutación 0,01</cx:v>
             </cx:txData>
           </cx:tx>
@@ -837,7 +807,7 @@
         <cx:series layoutId="boxWhisker" uniqueId="{29CBF583-4F27-471A-8FD7-2413BA363404}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.8</cx:f>
+              <cx:f>_xlchart.v1.10</cx:f>
               <cx:v>Mutación 0,05</cx:v>
             </cx:txData>
           </cx:tx>
@@ -850,13 +820,25 @@
         <cx:series layoutId="boxWhisker" uniqueId="{2ED0BBEE-508C-4D99-988B-81BB7E81C461}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:f>_xlchart.v1.12</cx:f>
               <cx:v>Mutación 0,09</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="2"/>
           <cx:layoutPr>
             <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{00000000-28F3-4C59-892B-BE6233E5D7E5}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:v>Mutación 0,00</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
@@ -882,17 +864,22 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.13</cx:f>
+        <cx:f>_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.15</cx:f>
+        <cx:f>_xlchart.v1.27</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.17</cx:f>
+        <cx:f>_xlchart.v1.29</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.31</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -916,10 +903,10 @@
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{69F4648F-678B-4CF2-815B-C3238B3764B1}">
+        <cx:series layoutId="boxWhisker" uniqueId="{16E52A3D-553F-4F8D-9E90-90427A9F17FB}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.12</cx:f>
+              <cx:f>_xlchart.v1.24</cx:f>
               <cx:v>Mutación 0,01</cx:v>
             </cx:txData>
           </cx:tx>
@@ -929,10 +916,10 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{4539CDDE-8C98-485C-8D36-E537F966E6E9}">
+        <cx:series layoutId="boxWhisker" uniqueId="{58708056-A2B7-4359-A808-6B9BB729512F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.14</cx:f>
+              <cx:f>_xlchart.v1.26</cx:f>
               <cx:v>Mutación 0,05</cx:v>
             </cx:txData>
           </cx:tx>
@@ -942,14 +929,27 @@
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{0499799E-DBD7-4A65-9E46-839655785097}">
+        <cx:series layoutId="boxWhisker" uniqueId="{117E479A-B023-4DCA-9D6F-5F266C75D5F6}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.16</cx:f>
+              <cx:f>_xlchart.v1.28</cx:f>
               <cx:v>Mutación 0,09</cx:v>
             </cx:txData>
           </cx:tx>
           <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{AAB3F599-A13B-4E13-B7FF-442AF9011D63}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.30</cx:f>
+              <cx:v>Mutación 0,00</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:dataId val="3"/>
           <cx:layoutPr>
             <cx:visibility meanLine="1" meanMarker="1" nonoutliers="0" outliers="1"/>
             <cx:statistics quartileMethod="exclusive"/>
@@ -3112,16 +3112,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -3180,16 +3180,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>200024</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>61911</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>419099</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>147635</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -3248,22 +3248,22 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>385762</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>61911</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="5" name="Gráfico 4"/>
+            <xdr:cNvPr id="6" name="Gráfico 5"/>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -3617,10 +3617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D6:T25"/>
+  <dimension ref="D6:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="J45" workbookViewId="0">
+      <selection activeCell="AC62" sqref="AC62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3632,7 +3632,7 @@
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="4:21" x14ac:dyDescent="0.25">
       <c r="R6" t="s">
         <v>6</v>
       </c>
@@ -3642,15 +3642,18 @@
       <c r="T6" t="s">
         <v>8</v>
       </c>
+      <c r="U6" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="7" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="1">
+    <row r="7" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E7">
         <v>20653</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7">
         <v>35859</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7">
         <v>4526</v>
       </c>
       <c r="I7">
@@ -3671,7 +3674,7 @@
       <c r="O7">
         <v>4488</v>
       </c>
-      <c r="R7" s="1">
+      <c r="R7">
         <v>20653</v>
       </c>
       <c r="S7">
@@ -3680,15 +3683,18 @@
       <c r="T7">
         <v>19944</v>
       </c>
+      <c r="U7">
+        <v>20526</v>
+      </c>
     </row>
-    <row r="8" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="1">
+    <row r="8" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E8">
         <v>20632</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8">
         <v>35869</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8">
         <v>4508</v>
       </c>
       <c r="I8">
@@ -3709,7 +3715,7 @@
       <c r="O8">
         <v>4428</v>
       </c>
-      <c r="R8" s="1">
+      <c r="R8">
         <v>20632</v>
       </c>
       <c r="S8">
@@ -3718,15 +3724,18 @@
       <c r="T8">
         <v>19874</v>
       </c>
+      <c r="U8">
+        <v>20349</v>
+      </c>
     </row>
-    <row r="9" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="1">
+    <row r="9" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E9">
         <v>20538</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9">
         <v>35801</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9">
         <v>4578</v>
       </c>
       <c r="I9">
@@ -3747,7 +3756,7 @@
       <c r="O9">
         <v>4466</v>
       </c>
-      <c r="R9" s="1">
+      <c r="R9">
         <v>20538</v>
       </c>
       <c r="S9">
@@ -3756,15 +3765,18 @@
       <c r="T9">
         <v>19907</v>
       </c>
+      <c r="U9">
+        <v>20576</v>
+      </c>
     </row>
-    <row r="10" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="1">
+    <row r="10" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E10">
         <v>20574</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10">
         <v>35742</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10">
         <v>4567</v>
       </c>
       <c r="I10">
@@ -3785,7 +3797,7 @@
       <c r="O10">
         <v>4447</v>
       </c>
-      <c r="R10" s="1">
+      <c r="R10">
         <v>20574</v>
       </c>
       <c r="S10">
@@ -3794,15 +3806,18 @@
       <c r="T10">
         <v>19785</v>
       </c>
+      <c r="U10">
+        <v>20506</v>
+      </c>
     </row>
-    <row r="11" spans="4:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E11" s="3">
+    <row r="11" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="E11">
         <v>20666</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11">
         <v>35730</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11">
         <v>4612</v>
       </c>
       <c r="I11">
@@ -3823,7 +3838,7 @@
       <c r="O11">
         <v>4478</v>
       </c>
-      <c r="R11" s="3">
+      <c r="R11">
         <v>20666</v>
       </c>
       <c r="S11">
@@ -3832,8 +3847,11 @@
       <c r="T11">
         <v>19809</v>
       </c>
+      <c r="U11">
+        <v>20445</v>
+      </c>
     </row>
-    <row r="13" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>0</v>
       </c>
@@ -3852,48 +3870,51 @@
       <c r="T13" t="s">
         <v>8</v>
       </c>
+      <c r="U13" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="14" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="1">
         <f>AVERAGE(E7:E11)</f>
         <v>20612.599999999999</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="1">
         <f>AVERAGE(F7:F11)</f>
         <v>35800.199999999997</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="1">
         <f>AVERAGE(G7:G11)</f>
         <v>4558.2</v>
       </c>
-      <c r="I14" s="5">
+      <c r="I14" s="1">
         <f>AVERAGE(I7:I11)</f>
         <v>20273.599999999999</v>
       </c>
-      <c r="J14" s="5">
+      <c r="J14" s="1">
         <f>AVERAGE(J7:J11)</f>
         <v>35077.599999999999</v>
       </c>
-      <c r="K14" s="5">
+      <c r="K14" s="1">
         <f>AVERAGE(K7:K11)</f>
         <v>4557.3999999999996</v>
       </c>
-      <c r="M14" s="5">
+      <c r="M14" s="1">
         <f>AVERAGE(M7:M11)</f>
         <v>19863.8</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="1">
         <f>AVERAGE(N7:N11)</f>
         <v>34446.800000000003</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="1">
         <f>AVERAGE(O7:O11)</f>
         <v>4461.3999999999996</v>
       </c>
-      <c r="R14" s="2">
+      <c r="R14">
         <v>35859</v>
       </c>
       <c r="S14">
@@ -3902,8 +3923,11 @@
       <c r="T14">
         <v>34510</v>
       </c>
+      <c r="U14">
+        <v>35583</v>
+      </c>
     </row>
-    <row r="15" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>4</v>
       </c>
@@ -3916,7 +3940,7 @@
       <c r="G15">
         <v>4557.3999999999996</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15">
         <v>35869</v>
       </c>
       <c r="S15">
@@ -3925,21 +3949,24 @@
       <c r="T15">
         <v>34433</v>
       </c>
+      <c r="U15">
+        <v>35629</v>
+      </c>
     </row>
-    <row r="16" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="1">
         <v>19863.8</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="1">
         <v>34446.800000000003</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="1">
         <v>4461.3999999999996</v>
       </c>
-      <c r="R16" s="2">
+      <c r="R16">
         <v>35801</v>
       </c>
       <c r="S16">
@@ -3948,9 +3975,12 @@
       <c r="T16">
         <v>34564</v>
       </c>
+      <c r="U16">
+        <v>35622</v>
+      </c>
     </row>
-    <row r="17" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R17" s="2">
+    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="R17">
         <v>35742</v>
       </c>
       <c r="S17">
@@ -3959,8 +3989,11 @@
       <c r="T17">
         <v>34291</v>
       </c>
+      <c r="U17">
+        <v>35505</v>
+      </c>
     </row>
-    <row r="18" spans="4:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>6</v>
       </c>
@@ -3970,7 +4003,7 @@
       <c r="G18" t="s">
         <v>8</v>
       </c>
-      <c r="R18" s="4">
+      <c r="R18">
         <v>35730</v>
       </c>
       <c r="S18">
@@ -3979,12 +4012,15 @@
       <c r="T18">
         <v>34436</v>
       </c>
+      <c r="U18">
+        <v>35553</v>
+      </c>
     </row>
-    <row r="19" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="1">
         <f>(STDEV(E14,L20)/L20)*100</f>
         <v>0.44451971396001938</v>
       </c>
@@ -3992,24 +4028,24 @@
         <f>(STDEV(E15,L20)/L20)*100</f>
         <v>1.6001346145155786</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="1">
         <f>(STDEV(E16,L20)/L20)*100</f>
         <v>2.9970991757181369</v>
       </c>
     </row>
-    <row r="20" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="1">
         <f>(STDEV(F14,M20)/M20)*100</f>
         <v>0.15923254067577575</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="1">
         <f>(STDEV(F15,M20)/M20)*100</f>
         <v>1.5832601878578447</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="1">
         <f>(STDEV(F16,M20)/M20)*100</f>
         <v>2.8263775969949121</v>
       </c>
@@ -4031,12 +4067,15 @@
       <c r="T20" t="s">
         <v>8</v>
       </c>
+      <c r="U20" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="21" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="1">
         <f>(STDEV(G14,N20)/N20)*100</f>
         <v>1.5150119528213306</v>
       </c>
@@ -4044,11 +4083,11 @@
         <f>(STDEV(G15,N20)/N20)*100</f>
         <v>1.5271563372126868</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="1">
         <f>(STDEV(G16,N20)/N20)*100</f>
         <v>2.9844824641750858</v>
       </c>
-      <c r="R21" s="1">
+      <c r="R21">
         <v>4526</v>
       </c>
       <c r="S21">
@@ -4057,9 +4096,12 @@
       <c r="T21">
         <v>4488</v>
       </c>
+      <c r="U21">
+        <v>4508</v>
+      </c>
     </row>
-    <row r="22" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R22" s="1">
+    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="R22">
         <v>4508</v>
       </c>
       <c r="S22">
@@ -4068,10 +4110,13 @@
       <c r="T22">
         <v>4428</v>
       </c>
+      <c r="U22">
+        <v>4462</v>
+      </c>
     </row>
-    <row r="23" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H23" s="6"/>
-      <c r="R23" s="1">
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="H23" s="2"/>
+      <c r="R23">
         <v>4578</v>
       </c>
       <c r="S23">
@@ -4080,9 +4125,12 @@
       <c r="T23">
         <v>4466</v>
       </c>
+      <c r="U23">
+        <v>4454</v>
+      </c>
     </row>
-    <row r="24" spans="4:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="R24" s="1">
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="R24">
         <v>4567</v>
       </c>
       <c r="S24">
@@ -4091,9 +4139,12 @@
       <c r="T24">
         <v>4447</v>
       </c>
+      <c r="U24">
+        <v>4498</v>
+      </c>
     </row>
-    <row r="25" spans="4:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="R25" s="3">
+    <row r="25" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="R25">
         <v>4612</v>
       </c>
       <c r="S25">
@@ -4101,6 +4152,9 @@
       </c>
       <c r="T25">
         <v>4478</v>
+      </c>
+      <c r="U25">
+        <v>4488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>